<commit_message>
[ADD] jpa config, insert data
</commit_message>
<xml_diff>
--- a/document/기능상세목록.xlsx
+++ b/document/기능상세목록.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
   <si>
     <t>기능명세</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -450,10 +450,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>POST  api/advertiser/signup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GET  api/advertiser/signin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -545,6 +541,36 @@
   </si>
   <si>
     <t>PUT  api/token/user/gifticon/{gift_id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>request</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>response</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST  api/advertiser/signup
+=&gt; Insert into Advertiser(~) values(~)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Advertiser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jwt header
+Advertiser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login
+{
+"email"
+"password"
+}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -741,29 +767,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1063,27 +1089,31 @@
     <col min="2" max="2" width="14.59765625" customWidth="1"/>
     <col min="3" max="3" width="26.3984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="75.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="104.69921875" customWidth="1"/>
-    <col min="6" max="6" width="32.8984375" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.8984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="104.69921875" customWidth="1"/>
+    <col min="8" max="8" width="32.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1097,403 +1127,469 @@
         <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:8" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="87" x14ac:dyDescent="0.4">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" ht="315" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21" t="s">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="315" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
+    <row r="9" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="12" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
+    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="16" t="s">
+      <c r="D14" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" ht="228" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" ht="228" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="H15" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="104.4" x14ac:dyDescent="0.4">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
+    <row r="16" spans="1:8" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="D16" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
+    <row r="17" spans="1:8" ht="61.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="D17" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
+    <row r="18" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" ht="82.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="21" t="s">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="82.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" ht="259.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21" t="s">
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="259.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
+    <row r="23" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21" t="s">
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27" t="s">
         <v>67</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>68</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
+    <row r="30" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="19" t="s">
         <v>69</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1501,7 +1597,7 @@
   <mergeCells count="8">
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="A19:A30"/>
-    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A5:A18"/>
     <mergeCell ref="B19:B21"/>

</xml_diff>

<commit_message>
[UPDATE] project merge update
</commit_message>
<xml_diff>
--- a/document/기능상세목록.xlsx
+++ b/document/기능상세목록.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>기능명세</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -450,6 +450,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>POST  api/advertiser/signup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>GET  api/advertiser/signin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -541,36 +545,6 @@
   </si>
   <si>
     <t>PUT  api/token/user/gifticon/{gift_id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>request</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>response</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POST  api/advertiser/signup
-=&gt; Insert into Advertiser(~) values(~)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Advertiser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jwt header
-Advertiser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Login
-{
-"email"
-"password"
-}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -767,6 +741,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -784,12 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1077,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1089,31 +1063,27 @@
     <col min="2" max="2" width="14.59765625" customWidth="1"/>
     <col min="3" max="3" width="26.3984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="75.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.8984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="104.69921875" customWidth="1"/>
-    <col min="8" max="8" width="32.8984375" customWidth="1"/>
+    <col min="5" max="5" width="104.69921875" customWidth="1"/>
+    <col min="6" max="6" width="32.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1127,469 +1097,403 @@
         <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="D5" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="87" x14ac:dyDescent="0.4">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="D6" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="7" t="s">
+      <c r="D7" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="315" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27" t="s">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="315" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="6" t="s">
+      <c r="D8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
+    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="12" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="6" t="s">
+      <c r="D10" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="7" t="s">
+      <c r="D11" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="8" t="s">
+      <c r="D12" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="16" t="s">
+      <c r="D13" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
+    <row r="14" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="16" t="s">
+      <c r="D14" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:8" ht="228" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" ht="228" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="6" t="s">
+      <c r="D15" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="104.4" x14ac:dyDescent="0.4">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
+    <row r="16" spans="1:6" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="10" t="s">
+      <c r="D16" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="61.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
+    <row r="17" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="10" t="s">
+      <c r="D17" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
+    <row r="18" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="6" t="s">
+      <c r="D18" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="82.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="27" t="s">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="82.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="6" t="s">
+      <c r="D21" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" ht="259.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27" t="s">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" ht="259.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="6" t="s">
+      <c r="D22" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
+    <row r="23" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27" t="s">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>68</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
+    <row r="30" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="19" t="s">
         <v>69</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1597,7 +1501,7 @@
   <mergeCells count="8">
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="A19:A30"/>
-    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A5:A18"/>
     <mergeCell ref="B19:B21"/>

</xml_diff>